<commit_message>
Finished real time monitoring
</commit_message>
<xml_diff>
--- a/Cahier de charge.xlsx
+++ b/Cahier de charge.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YAHYAX\Workspace\Projects\CYBERSEC\SYSGUARD\SYSGUARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7BDC55-D99C-4D62-865C-FB41E173523D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4387C4B-CD28-4516-B770-8FD2CD42D059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{D3BBEA7B-0041-42A8-BFC3-0FD19AF0C7B4}"/>
   </bookViews>
@@ -81,14 +81,14 @@
     <t>Automatic Ban (Black list)</t>
   </si>
   <si>
-    <t>Live mode monitoring</t>
+    <t>Subshell -s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,8 +111,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,6 +141,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -165,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -183,10 +196,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -506,7 +522,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -599,17 +615,17 @@
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="7"/>
     </row>
     <row r="15" spans="1:2" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="7"/>
+      <c r="B15" s="9"/>
     </row>
     <row r="16" spans="1:2" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
+      <c r="B16" s="8"/>
     </row>
     <row r="17" spans="1:2" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="3"/>

</xml_diff>